<commit_message>
Chap6 : Analyse sensibilité : analyse visuelle
</commit_message>
<xml_diff>
--- a/chap6/src/AnalyseSensibilite/0_src/Parametres.xlsx
+++ b/chap6/src/AnalyseSensibilite/0_src/Parametres.xlsx
@@ -11,8 +11,16 @@
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Feuille3" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="inputs" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Selection" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Table dynamique_Selection_1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Selection!$A$1:$H$15</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <pivotCaches>
+    <pivotCache cacheId="1" r:id="rId8"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="280">
   <si>
     <t xml:space="preserve">INPUTS (12)</t>
   </si>
@@ -371,7 +379,7 @@
     <t xml:space="preserve">Date à partir de laquelle des châteaux peuvent être construits par les seigneurs</t>
   </si>
   <si>
-    <t xml:space="preserve">distance_detection_agregat</t>
+    <t xml:space="preserve">debut_construction_chateaux</t>
   </si>
   <si>
     <t xml:space="preserve">[820, 880, 940, 1000, 1060]</t>
@@ -487,6 +495,9 @@
     <t xml:space="preserve">Distance maximale entre les foyers paysans et les attracteurs les plus proches pour qu'ils soient considérés comme faisant partie d'un même agrégat</t>
   </si>
   <si>
+    <t xml:space="preserve">distance_detection_agregat</t>
+  </si>
+  <si>
     <t xml:space="preserve">100 m.</t>
   </si>
   <si>
@@ -726,7 +737,7 @@
     <t xml:space="preserve">Nombre minimum de foyers paysans insatisfaits requis pour la création d'une nouvelle église paroissiale en-dehors d'un agrégat</t>
   </si>
   <si>
-    <t xml:space="preserve">seuil_nb_paroissiens_insatisfaits</t>
+    <t xml:space="preserve">_</t>
   </si>
   <si>
     <t xml:space="preserve">[5, 10, 20, 30, 50]</t>
@@ -1958,9 +1969,6 @@
     <t xml:space="preserve">Paramètres de contexte : 13 params, 12 à tester</t>
   </si>
   <si>
-    <t xml:space="preserve">debut_construction_chateaux</t>
-  </si>
-  <si>
     <t xml:space="preserve">Paramètres de mécanisme : 31 params, 23 ensemble à tester</t>
   </si>
   <si>
@@ -1978,6 +1986,9 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">seuil_nb_paroissiens_insatisfaits</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paramètres techniques : 11 params, 11 à tester</t>
   </si>
   <si>
@@ -1991,6 +2002,109 @@
   </si>
   <si>
     <t xml:space="preserve">Églises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type de paramètre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agents caractérisés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valeurs testées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origine de la sélection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rang sensibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Étendue (variable au cours du temps) dans laquelle un foyer paysan calcule sa satisfaction religieuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_minmax_eglise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mécanisme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avant 960 : de 5km à 25km
+Entre 960 et 1060 : de 3 à 10km
+Après 1060 : de 1.5 à 5km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Valeur par défaut : base
+- Entre 5km et 25km tout au long : statique_large
+- Entre 1.5km et 5km tout au long : statique_reduit
+- Avant 960 : [1.5, 5], de 960 à 1060 : [1, 3], après : [0.5, 1.5] : dynamique_reduit
+- Avant 960 : [25, 50], de 960 à 1060 : [10, 25], après : [5, 10] : dynamique_large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Globale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrégats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0, 0.5, 1, 1.5, 2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[800::2500] : 2500m tout au long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- 2500m tout au long : base
+- 1000m tout au long : statique_reduit
+- 2500m jusqu’à 1000, puis 5000m : dyn_croissant
+- 1000m jusqu’en 1000, puis 2500m : dyn_reduit
+- 5000m jusqu’en 1000, puis 10000m : dyn_large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contexte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 tout au long : statique_nul
+1 tout au long : statique_fort
+Graduel défaut : base
+0 + 0.1/an à partir de 900 : croissant_regulier
+0 avant 1000, puis 0.5 : croissant_seuil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio_charge_fiscale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0, 1, 2, 3, 4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nb_grands_chateaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance_eglises_paroissiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avec variation pop_init , pour pop 40k final constante :
+croissance_demo : 0.0 &amp; init_nb_total_fp : 40000
+croissance_demo : 0.1289 &amp; init_nb_total_fp : 4000
+croissance_demo : 0.0589 &amp; init_nb_total_fp : 13500
+croissance_demo : 0.0372 &amp; init_nb_total_fp : 20000
+croissance_demo : 0.0153 &amp; init_nb_total_fp : 30000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compter - Intitulé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Données</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Résultat</t>
   </si>
 </sst>
 </file>
@@ -2000,7 +2114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2080,8 +2194,35 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="10"/>
+      <name val="Charis SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Charis SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Charis SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Charis SIL"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2100,8 +2241,14 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729FCF"/>
+        <bgColor rgb="FF888A85"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="30">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -2144,8 +2291,176 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2169,8 +2484,26 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="96">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2247,23 +2580,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2327,14 +2648,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2387,14 +2700,208 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="22" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="24" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="25" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="26" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="27" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="28" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="29" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Coin de la table dynamique" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Valeur de la table dynamique" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Champ de la table dynamique" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Catégorie de la table dynamique" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Titre de la table dynamique" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Résultat de la table dynamique" xfId="25" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2414,7 +2921,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF7D7D7D"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
@@ -2459,6 +2966,168 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" recordCount="14" createdVersion="3">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:D15" sheet="Selection"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Intitulé" numFmtId="0">
+      <sharedItems count="14">
+        <s v="croissance_demo"/>
+        <s v="debut_construction_chateaux"/>
+        <s v="dist_minmax_eglise"/>
+        <s v="distance_detection_agregat"/>
+        <s v="droits_fonciers_zp"/>
+        <s v="nb_min_fp_agregat"/>
+        <s v="nb_tirages_chateaux_ps"/>
+        <s v="periode_promotion_chateaux"/>
+        <s v="ponderation_creation_paroisse_agregat"/>
+        <s v="proba_creation_zp_autres_droits_ps"/>
+        <s v="proba_gain_haute_justice_gs"/>
+        <s v="rayon_migration_locale_fp"/>
+        <s v="taille_cote_monde"/>
+        <s v="taux_prelevement_zp_chateau"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Type de paramètre" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Contexte"/>
+        <s v="Input"/>
+        <s v="Mécanisme"/>
+        <s v="Technique"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Agents caractérisés" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Agrégats"/>
+        <s v="Châteaux"/>
+        <s v="Églises"/>
+        <s v="Foyers paysans"/>
+        <s v="Monde"/>
+        <s v="Seigneurs"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="14">
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="1"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="Values" useAutoFormatting="0" itemPrintTitles="1" indent="0" outline="0" outlineData="0" compact="0" compactData="0">
+  <location ref="A1:H7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0" compact="0" outline="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0" compact="0" outline="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0" compact="0" outline="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <colFields count="2">
+    <field x="-2"/>
+    <field x="2"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField fld="0" subtotal="count"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -2466,15 +3135,15 @@
   </sheetPr>
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="77.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.71"/>
   </cols>
@@ -2770,19 +3439,19 @@
       <c r="D23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="19" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3061,7 +3730,7 @@
       <c r="D44" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3076,7 +3745,7 @@
         <v>102</v>
       </c>
       <c r="D45" s="17"/>
-      <c r="E45" s="23"/>
+      <c r="E45" s="20"/>
     </row>
     <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="7" t="s">
@@ -3091,7 +3760,7 @@
       <c r="D46" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3106,7 +3775,7 @@
         <v>109</v>
       </c>
       <c r="D47" s="17"/>
-      <c r="E47" s="23"/>
+      <c r="E47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="7" t="s">
@@ -3118,7 +3787,7 @@
       <c r="C48" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="21" t="s">
         <v>113</v>
       </c>
       <c r="E48" s="0" t="s">
@@ -3135,7 +3804,7 @@
       <c r="C49" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="D49" s="21" t="s">
         <v>116</v>
       </c>
       <c r="E49" s="0" t="s">
@@ -3160,7 +3829,7 @@
       <c r="C51" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="D51" s="24" t="s">
+      <c r="D51" s="21" t="s">
         <v>119</v>
       </c>
       <c r="E51" s="0" t="s">
@@ -3172,13 +3841,13 @@
         <v>120</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" s="24" t="s">
         <v>122</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>10</v>
@@ -3191,54 +3860,54 @@
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="10"/>
-      <c r="E53" s="25"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D54" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="D54" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D55" s="24" t="s">
         <v>130</v>
       </c>
+      <c r="D55" s="21" t="s">
+        <v>131</v>
+      </c>
       <c r="E55" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="24" t="s">
         <v>134</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>135</v>
       </c>
       <c r="E56" s="0" t="s">
         <v>10</v>
@@ -3246,16 +3915,16 @@
     </row>
     <row r="57" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D57" s="26" t="s">
         <v>138</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>50</v>
@@ -3263,16 +3932,16 @@
     </row>
     <row r="58" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="D58" s="27" t="s">
         <v>142</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>143</v>
       </c>
       <c r="E58" s="0" t="s">
         <v>50</v>
@@ -3280,16 +3949,16 @@
     </row>
     <row r="59" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D59" s="24" t="s">
         <v>146</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>147</v>
       </c>
       <c r="E59" s="0" t="s">
         <v>10</v>
@@ -3297,16 +3966,16 @@
     </row>
     <row r="60" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D60" s="24" t="s">
         <v>150</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="E60" s="0" t="s">
         <v>10</v>
@@ -3314,16 +3983,16 @@
     </row>
     <row r="61" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D61" s="24" t="s">
         <v>154</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>155</v>
       </c>
       <c r="E61" s="0" t="s">
         <v>10</v>
@@ -3331,16 +4000,16 @@
     </row>
     <row r="62" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="7" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="D62" s="24" t="s">
-        <v>126</v>
+        <v>158</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>10</v>
@@ -3348,16 +4017,16 @@
     </row>
     <row r="63" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D63" s="24" t="s">
         <v>126</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="E63" s="0" t="s">
         <v>10</v>
@@ -3373,16 +4042,16 @@
     </row>
     <row r="65" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C65" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E65" s="0" t="s">
         <v>50</v>
@@ -3390,16 +4059,16 @@
     </row>
     <row r="66" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="D66" s="24" t="s">
         <v>167</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="E66" s="0" t="s">
         <v>10</v>
@@ -3407,16 +4076,16 @@
     </row>
     <row r="67" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D67" s="24" t="s">
-        <v>126</v>
+        <v>171</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="E67" s="0" t="s">
         <v>10</v>
@@ -3424,16 +4093,16 @@
     </row>
     <row r="68" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="7" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C68" s="16" t="s">
-        <v>173</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>126</v>
+        <v>174</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="E68" s="0" t="s">
         <v>10</v>
@@ -3441,7 +4110,7 @@
     </row>
     <row r="69" customFormat="false" ht="13.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -3449,33 +4118,33 @@
     </row>
     <row r="70" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C70" s="16" t="n">
         <v>2000</v>
       </c>
-      <c r="D70" s="24" t="s">
-        <v>177</v>
+      <c r="D70" s="21" t="s">
+        <v>178</v>
       </c>
       <c r="E70" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C71" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="D71" s="24" t="s">
-        <v>180</v>
+      <c r="D71" s="21" t="s">
+        <v>181</v>
       </c>
       <c r="E71" s="0" t="s">
         <v>10</v>
@@ -3483,7 +4152,7 @@
     </row>
     <row r="72" customFormat="false" ht="13.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -3491,102 +4160,102 @@
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C73" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="E73" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="E73" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D74" s="17"/>
-      <c r="E74" s="23"/>
+      <c r="E74" s="20"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D75" s="17"/>
-      <c r="E75" s="23"/>
+      <c r="E75" s="20"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C76" s="16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D76" s="17"/>
-      <c r="E76" s="23"/>
+      <c r="E76" s="20"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D77" s="17"/>
-      <c r="E77" s="23"/>
+      <c r="E77" s="20"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D78" s="17"/>
-      <c r="E78" s="23"/>
+      <c r="E78" s="20"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D79" s="17"/>
-      <c r="E79" s="23"/>
+      <c r="E79" s="20"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B80" s="18"/>
       <c r="C80" s="18"/>
@@ -3620,10 +4289,10 @@
     </row>
     <row r="84" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C84" s="16" t="n">
         <v>15</v>
@@ -3637,16 +4306,16 @@
     </row>
     <row r="85" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C85" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E85" s="0" t="s">
         <v>10</v>
@@ -3662,16 +4331,16 @@
     </row>
     <row r="87" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D87" s="28" t="s">
-        <v>210</v>
+        <v>122</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>211</v>
       </c>
       <c r="E87" s="0" t="s">
         <v>10</v>
@@ -3687,16 +4356,16 @@
     </row>
     <row r="89" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C89" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="D89" s="29" t="s">
-        <v>213</v>
+      <c r="D89" s="26" t="s">
+        <v>214</v>
       </c>
       <c r="E89" s="0" t="s">
         <v>10</v>
@@ -3704,16 +4373,16 @@
     </row>
     <row r="90" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="D90" s="28" t="s">
         <v>217</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="E90" s="0" t="s">
         <v>10</v>
@@ -3721,16 +4390,16 @@
     </row>
     <row r="91" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C91" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D91" s="28" t="s">
-        <v>220</v>
+      <c r="D91" s="25" t="s">
+        <v>221</v>
       </c>
       <c r="E91" s="0" t="s">
         <v>10</v>
@@ -3738,16 +4407,16 @@
     </row>
     <row r="92" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="D92" s="28" t="s">
         <v>224</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>225</v>
       </c>
       <c r="E92" s="0" t="s">
         <v>10</v>
@@ -3755,16 +4424,16 @@
     </row>
     <row r="93" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="D93" s="28" t="s">
-        <v>227</v>
+        <v>189</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>228</v>
       </c>
       <c r="E93" s="0" t="s">
         <v>10</v>
@@ -3772,16 +4441,16 @@
     </row>
     <row r="94" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="D94" s="28" t="s">
         <v>231</v>
+      </c>
+      <c r="D94" s="25" t="s">
+        <v>232</v>
       </c>
       <c r="E94" s="0" t="s">
         <v>10</v>
@@ -3789,16 +4458,16 @@
     </row>
     <row r="95" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="7" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C95" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="D95" s="28" t="s">
-        <v>234</v>
+      <c r="D95" s="25" t="s">
+        <v>235</v>
       </c>
       <c r="E95" s="0" t="s">
         <v>10</v>
@@ -3806,16 +4475,16 @@
     </row>
     <row r="96" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C96" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="D96" s="28" t="s">
-        <v>237</v>
+      <c r="D96" s="25" t="s">
+        <v>238</v>
       </c>
       <c r="E96" s="0" t="s">
         <v>10</v>
@@ -3885,7 +4554,7 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -3897,25 +4566,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30" t="s">
-        <v>238</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="33" t="n">
+      <c r="C3" s="30" t="n">
         <v>80</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -3923,13 +4592,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="33" t="n">
+      <c r="C4" s="30" t="n">
         <v>50000</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -3937,13 +4606,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="33" t="n">
+      <c r="C5" s="30" t="n">
         <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -3951,13 +4620,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="33" t="n">
+      <c r="C6" s="30" t="n">
         <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -3965,13 +4634,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="33" t="n">
+      <c r="C7" s="30" t="n">
         <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
@@ -3979,13 +4648,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="33" t="n">
+      <c r="C8" s="30" t="n">
         <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
@@ -3993,36 +4662,36 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="36" t="n">
+      <c r="C9" s="33" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="33" t="n">
+      <c r="C11" s="30" t="n">
         <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -4030,13 +4699,13 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="33" t="n">
+      <c r="C12" s="30" t="n">
         <v>150</v>
       </c>
       <c r="D12" s="0" t="s">
@@ -4044,13 +4713,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="33" t="n">
+      <c r="C13" s="30" t="n">
         <v>50</v>
       </c>
       <c r="D13" s="0" t="s">
@@ -4058,37 +4727,37 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37" t="s">
-        <v>239</v>
-      </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
+      <c r="A14" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
     </row>
     <row r="16" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="24" t="s">
         <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -4096,13 +4765,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="0" t="s">
@@ -4110,13 +4779,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="165.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="24" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
@@ -4124,13 +4793,13 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="178.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="24" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="0" t="s">
@@ -4138,13 +4807,13 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="24" t="s">
         <v>57</v>
       </c>
       <c r="D21" s="0" t="s">
@@ -4152,704 +4821,704 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="27" t="n">
+      <c r="C22" s="24" t="n">
         <v>200</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="27" t="n">
+      <c r="C25" s="24" t="n">
         <v>880</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="27" t="n">
+      <c r="C26" s="24" t="n">
         <v>960</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C27" s="27" t="n">
+      <c r="B27" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="24" t="n">
         <v>940</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="19" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="39"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="39"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="20" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="114.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="20" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="24" t="s">
         <v>243</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="39" t="s">
+      <c r="D36" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="27" t="n">
+      <c r="C37" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="D37" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B38" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="27" t="s">
+      <c r="B38" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="C38" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="B39" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="C39" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D39" s="22" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" s="31" t="s">
+      <c r="A40" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="C40" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="39" t="s">
+      <c r="C40" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" s="31" t="s">
+      <c r="A41" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="B41" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="C41" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="31" t="s">
+      <c r="A42" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="B42" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="C42" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="B43" s="31" t="s">
+      <c r="A43" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="B43" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="C43" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="B44" s="31" t="s">
+      <c r="A44" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="B44" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="C44" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" s="31" t="s">
+      <c r="A45" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="B45" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="D45" s="39" t="s">
+      <c r="C45" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="B46" s="31" t="s">
+      <c r="A46" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="B46" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="D46" s="39" t="s">
+      <c r="C46" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="127.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="31" t="s">
+      <c r="A47" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="B47" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="C47" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="B48" s="31" t="s">
+      <c r="A48" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="C48" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="D48" s="39" t="s">
+      <c r="B48" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="B49" s="31" t="s">
+      <c r="A49" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="B49" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="C49" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="B50" s="31" t="s">
+      <c r="A50" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="C50" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="39" t="s">
+      <c r="C50" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="31" t="s">
+      <c r="A51" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="B51" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="C51" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="B52" s="31" t="s">
+      <c r="A52" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="C52" s="27" t="s">
+      <c r="B52" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D52" s="39" t="s">
+      <c r="C52" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="B53" s="31" t="s">
+      <c r="A53" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="C53" s="27" t="n">
+      <c r="B53" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="24" t="n">
         <v>2000</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="B54" s="31" t="s">
+      <c r="A54" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="C54" s="27" t="n">
+      <c r="B54" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="C54" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="B55" s="31" t="s">
+      <c r="A55" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="B55" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="C55" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" s="31" t="s">
+      <c r="A56" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="B56" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="D56" s="40"/>
+      <c r="C56" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="20"/>
     </row>
     <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="31" t="s">
+      <c r="A57" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="20"/>
+    </row>
+    <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="C58" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="B57" s="31" t="s">
-        <v>190</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="D57" s="40"/>
-    </row>
-    <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="B58" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="D58" s="40"/>
+      <c r="D58" s="20"/>
     </row>
     <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="B59" s="31" t="s">
+      <c r="A59" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="C59" s="27" t="s">
+      <c r="B59" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="D59" s="40"/>
+      <c r="C59" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59" s="20"/>
     </row>
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="B60" s="31" t="s">
+      <c r="A60" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="B60" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="D60" s="40"/>
+      <c r="C60" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D60" s="20"/>
     </row>
     <row r="61" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="31" t="s">
-        <v>199</v>
-      </c>
-      <c r="B61" s="31" t="s">
+      <c r="A61" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="C61" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="D61" s="40"/>
+      <c r="B61" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D61" s="20"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="37" t="s">
-        <v>246</v>
-      </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="39"/>
+      <c r="A62" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="37"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
-      <c r="D63" s="39"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="19"/>
     </row>
     <row r="64" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="B64" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="C64" s="27" t="n">
+      <c r="A64" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="C64" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="D64" s="39" t="s">
+      <c r="D64" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="B65" s="31" t="s">
+      <c r="A65" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="C65" s="27" t="s">
+      <c r="B65" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="D65" s="39" t="s">
+      <c r="C65" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D65" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" s="31" t="s">
+      <c r="A66" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C66" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="D66" s="39" t="s">
+      <c r="B66" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="B67" s="31" t="s">
+      <c r="A67" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="C67" s="27" t="n">
+      <c r="B67" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="D67" s="39" t="s">
+      <c r="D67" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="31" t="s">
-        <v>214</v>
-      </c>
-      <c r="B68" s="31" t="s">
+      <c r="A68" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="B68" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="D68" s="39" t="s">
+      <c r="C68" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="D68" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="B69" s="31" t="s">
+      <c r="A69" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="C69" s="27" t="n">
+      <c r="B69" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D69" s="39" t="s">
+      <c r="D69" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="B70" s="31" t="s">
+      <c r="A70" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C70" s="27" t="s">
+      <c r="B70" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="D70" s="39" t="s">
+      <c r="C70" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="63.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="31" t="s">
-        <v>225</v>
-      </c>
-      <c r="B71" s="31" t="s">
+      <c r="A71" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="C71" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="D71" s="39" t="s">
+      <c r="B71" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="31" t="s">
-        <v>228</v>
-      </c>
-      <c r="B72" s="31" t="s">
+      <c r="A72" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C72" s="27" t="s">
+      <c r="B72" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="D72" s="39" t="s">
+      <c r="C72" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D72" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="31" t="s">
-        <v>232</v>
-      </c>
-      <c r="B73" s="31" t="s">
+      <c r="A73" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="C73" s="27" t="n">
+      <c r="B73" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="D73" s="39" t="s">
+      <c r="D73" s="19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="B74" s="31" t="s">
+      <c r="A74" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="C74" s="27" t="n">
+      <c r="B74" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D74" s="39" t="s">
+      <c r="D74" s="19" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4880,7 +5549,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -4889,214 +5558,216 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
-        <v>248</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="A1" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>249</v>
-      </c>
-      <c r="B3" s="42" t="s">
+      <c r="A3" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="76.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="46" t="n">
+      <c r="D4" s="41" t="n">
         <v>80</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="42" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="46" t="n">
+      <c r="D5" s="41" t="n">
         <v>50000</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="46" t="n">
+      <c r="D6" s="41" t="n">
         <v>8</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="42" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="46" t="n">
+      <c r="D7" s="41" t="n">
         <v>30</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="42" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="46" t="n">
+      <c r="D8" s="41" t="n">
         <v>20</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="46" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="50" t="n">
+      <c r="D10" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="46" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="53" t="s">
+      <c r="E11" s="48" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44" t="s">
+      <c r="A12" s="38"/>
+      <c r="B12" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="46" t="n">
+      <c r="D12" s="41" t="n">
         <v>18</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43" t="s">
-        <v>250</v>
-      </c>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="46" t="n">
+      <c r="D13" s="41" t="n">
         <v>150</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="46" t="n">
+      <c r="D14" s="41" t="n">
         <v>50</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="42" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5115,4 +5786,600 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="35.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="50" width="10.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="57.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="49" width="10"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="52" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>261</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H2" s="54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" s="61" t="n">
+        <v>80</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H3" s="60" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>265</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H4" s="54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" s="60" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>268</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>269</v>
+      </c>
+      <c r="G6" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="54" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H7" s="60" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="55" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F8" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H8" s="54" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>271</v>
+      </c>
+      <c r="G9" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H9" s="60" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="55" t="n">
+        <v>940</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>262</v>
+      </c>
+      <c r="H10" s="54" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>265</v>
+      </c>
+      <c r="E11" s="61" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="H11" s="60" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="57" t="s">
+        <v>272</v>
+      </c>
+      <c r="H12" s="54" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" s="60" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="62" t="s">
+        <v>273</v>
+      </c>
+      <c r="G13" s="63" t="s">
+        <v>274</v>
+      </c>
+      <c r="H13" s="60" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>275</v>
+      </c>
+      <c r="H14" s="54" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="61" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="62" t="s">
+        <v>276</v>
+      </c>
+      <c r="G15" s="63" t="s">
+        <v>272</v>
+      </c>
+      <c r="H15" s="60" t="n">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H15"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="72" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="64" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="68" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="70" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="74" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="77" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="78" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="82"/>
+      <c r="H4" s="83" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="78" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" s="84" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="80"/>
+      <c r="D5" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="81" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="80"/>
+      <c r="G5" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="83" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="78" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="86"/>
+      <c r="C6" s="87" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="89" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="90" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="91" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="92" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="93" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="93" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="93" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="94" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="95" t="n">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Chap6 : fin analyse sensibilité (sensibilité aléa + conclusion)
</commit_message>
<xml_diff>
--- a/chap6/src/AnalyseSensibilite/0_src/Parametres.xlsx
+++ b/chap6/src/AnalyseSensibilite/0_src/Parametres.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
     <sheet name="Table dynamique_Selection_1" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Selection!$A$1:$H$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Selection!$A$1:$H$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <pivotCaches>
@@ -2196,8 +2196,8 @@
     </font>
     <font>
       <b val="true"/>
-      <i val="true"/>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Charis SIL"/>
       <family val="0"/>
       <charset val="1"/>
@@ -2222,7 +2222,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2243,8 +2243,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF729FCF"/>
-        <bgColor rgb="FF888A85"/>
+        <fgColor rgb="FF414487"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBEBEB"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -2736,27 +2742,27 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2921,9 +2927,9 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF7D7D7D"/>
-      <rgbColor rgb="FF729FCF"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFEBEBEB"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -2945,7 +2951,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3333FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -2959,15 +2965,11 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF3333FF"/>
+      <rgbColor rgb="FF414487"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3135,7 +3137,7 @@
   </sheetPr>
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -4554,7 +4556,7 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -5549,7 +5551,7 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -5795,24 +5797,24 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="35.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="34.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="35.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="50" width="10.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="50" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="57.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="59.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="24.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="49" width="10"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="34.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="51" t="s">
         <v>1</v>
       </c>
@@ -5890,7 +5892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="59.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="52" t="s">
         <v>120</v>
       </c>
@@ -5916,7 +5918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="58" t="s">
         <v>219</v>
       </c>
@@ -6124,7 +6126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="32.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="58" t="s">
         <v>236</v>
       </c>
@@ -6203,7 +6205,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H15"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="72" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6211,7 +6212,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6222,7 +6222,7 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>